<commit_message>
# 작업 기간 - 2025-06-01 ~ 2025-06-08
# 커밋 내용
- 기안 작성 목록 화면 개발
- 휴가 신청서, 가지급결의서, 물품반출입신청서, 법인카드 정산서 작성 상세 화면 개발
- 물품 등록, 조회 팝업 개발
- 정산내역 등록, 조회 팝업 개발
- 프로필 사진 영역 사이즈 변경
- 프로필 사진 삭제 후 재 로드 시 나오지 않는 문제 수정
- 모달 창 동작 시 오버레이 처리
- 모달 창 동작 로직 수정 (obj에 담는 방식으로)
- 결재선 등록, 조회 화면 리뉴얼 (조회 화면 내 결재의견 조회란 추가 등)
- 스크롤 생성 시, 상단 메뉴가 스크롤 너비 만큼 이동하는 문제 수정
- select박스 (div) 가 모달창과 메인화면에서 기능이 겹쳐 동작하지 않는 문제 수정
- 트랜젝션 어노테이션 추가
</commit_message>
<xml_diff>
--- a/02.프로젝트/01.인트라넷/01.설계/인트라넷 데이터.xlsx
+++ b/02.프로젝트/01.인트라넷/01.설계/인트라넷 데이터.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knn\Documents\hikr90\02.프로젝트\01.인트라넷\01.설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0C140C-EEE1-4C54-B229-D2AABDE35604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE7C38-9BBD-497E-9645-ADAC89AA8220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="793" activeTab="7" xr2:uid="{B204C4DA-9ED1-4F0A-AC7E-C11DE778500E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="213">
   <si>
     <t>EMP_IDX</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -203,9 +203,6 @@
     <t>intrAprvInqy2010.do</t>
   </si>
   <si>
-    <t>업무관리</t>
-  </si>
-  <si>
     <t>intrTaskInqy1010.do</t>
   </si>
   <si>
@@ -218,398 +215,582 @@
     <t>intrEmpInqy2010.do</t>
   </si>
   <si>
+    <t>공지사항 관리</t>
+  </si>
+  <si>
+    <t>업무일지 조회</t>
+  </si>
+  <si>
+    <t>intrTaskInqy2010.do</t>
+  </si>
+  <si>
+    <t>결재 관리</t>
+  </si>
+  <si>
+    <t>intrTempInqy1010.do</t>
+  </si>
+  <si>
+    <t>사원 관리</t>
+  </si>
+  <si>
+    <t>intrEmpInqy1010.do</t>
+  </si>
+  <si>
+    <t>시스템 관리</t>
+  </si>
+  <si>
+    <t>권한 관리</t>
+  </si>
+  <si>
+    <t>intrAuthInqy1010.do</t>
+  </si>
+  <si>
+    <t>메뉴 권한 부여</t>
+  </si>
+  <si>
+    <t>intrAuthInqy2010.do</t>
+  </si>
+  <si>
+    <t>사용자 권한 부여</t>
+  </si>
+  <si>
+    <t>intrAuthInqy3010.do</t>
+  </si>
+  <si>
+    <t>MENU_0022</t>
+  </si>
+  <si>
+    <t>쿼리 입력</t>
+  </si>
+  <si>
+    <t>intrQueryInqy1010.do</t>
+  </si>
+  <si>
+    <t>MENU_0023</t>
+  </si>
+  <si>
+    <t>MENU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUTH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrProjInqy1010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUTH_0002</t>
+  </si>
+  <si>
+    <t>테스트 권한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENU_AUTH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP_AUTH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMPINFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORG_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RANK_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IS_MALE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOB_NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_INFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMAIL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HIRE_DT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEAV_DT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP_0001</t>
+  </si>
+  <si>
+    <t>ORG_0001</t>
+  </si>
+  <si>
+    <t>RANK_0001</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>주소</t>
+  </si>
+  <si>
+    <t>jtax90@naver.com</t>
+  </si>
+  <si>
+    <t>01077945147</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORG_NM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPPR_ORG_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORG_0002</t>
+  </si>
+  <si>
+    <t>ORG_0003</t>
+  </si>
+  <si>
+    <t>ORG_0004</t>
+  </si>
+  <si>
+    <t>000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RANK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+  </si>
+  <si>
+    <t>RANK_0002</t>
+  </si>
+  <si>
+    <t>RANK_0003</t>
+  </si>
+  <si>
+    <t>RANK_NM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RANK_0004</t>
+  </si>
+  <si>
+    <t>RANK_0005</t>
+  </si>
+  <si>
+    <t>RANK_0006</t>
+  </si>
+  <si>
+    <t>RANK_0007</t>
+  </si>
+  <si>
+    <t>RANK_0008</t>
+  </si>
+  <si>
+    <t>RANK_0009</t>
+  </si>
+  <si>
+    <t>RANK_0010</t>
+  </si>
+  <si>
+    <t>ORG_0005</t>
+  </si>
+  <si>
+    <t>ORG_0006</t>
+  </si>
+  <si>
+    <t>ORG_0007</t>
+  </si>
+  <si>
+    <t>ORG_0008</t>
+  </si>
+  <si>
+    <t>ORG_0009</t>
+  </si>
+  <si>
+    <t>ORG_0010</t>
+  </si>
+  <si>
+    <t>ORG_0011</t>
+  </si>
+  <si>
+    <t>경영지원부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재무/회계부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마케팅부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영업부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생산부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구개발부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객지원팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보시스템팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>품질관리부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>법무팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORG_0012</t>
+  </si>
+  <si>
+    <t>ORG_0013</t>
+  </si>
+  <si>
+    <t>COMMCODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMCODE_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMCODE_NM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMCODE_GCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>결재 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결재선 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행</t>
+  </si>
+  <si>
+    <t>완료</t>
+  </si>
+  <si>
+    <t>보류</t>
+  </si>
+  <si>
+    <t>기안 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양식 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENU_0024</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAQ 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메일 전송</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부서/직급 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENU_0025</t>
+  </si>
+  <si>
+    <t>MENU_0026</t>
+  </si>
+  <si>
+    <t>MENU_0027</t>
+  </si>
+  <si>
+    <t>MENU_0028</t>
+  </si>
+  <si>
+    <t>업무일지 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrAprvInqy3010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrFaqInqy2010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrFaqInqy1010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrMailInqy1010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrRoleInqy1010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무일지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENU_0029</t>
+  </si>
+  <si>
+    <t>MENU_0030</t>
+  </si>
+  <si>
+    <t>MENU_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잔여휴가 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>병가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경조휴가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>공유정보 관리</t>
-  </si>
-  <si>
-    <t>공지사항 관리</t>
-  </si>
-  <si>
-    <t>업무일지 조회</t>
-  </si>
-  <si>
-    <t>intrTaskInqy2010.do</t>
-  </si>
-  <si>
-    <t>결재 관리</t>
-  </si>
-  <si>
-    <t>기안문 관리</t>
-  </si>
-  <si>
-    <t>intrTempInqy1010.do</t>
-  </si>
-  <si>
-    <t>사원 관리</t>
-  </si>
-  <si>
-    <t>intrEmpInqy1010.do</t>
-  </si>
-  <si>
-    <t>시스템 관리</t>
-  </si>
-  <si>
-    <t>권한 관리</t>
-  </si>
-  <si>
-    <t>intrAuthInqy1010.do</t>
-  </si>
-  <si>
-    <t>메뉴 권한 부여</t>
-  </si>
-  <si>
-    <t>intrAuthInqy2010.do</t>
-  </si>
-  <si>
-    <t>사용자 권한 부여</t>
-  </si>
-  <si>
-    <t>intrAuthInqy3010.do</t>
-  </si>
-  <si>
-    <t>MENU_0022</t>
-  </si>
-  <si>
-    <t>쿼리 입력</t>
-  </si>
-  <si>
-    <t>intrQueryInqy1010.do</t>
-  </si>
-  <si>
-    <t>MENU_0023</t>
-  </si>
-  <si>
-    <t>MENU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intrProjInqy1010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUTH_0002</t>
-  </si>
-  <si>
-    <t>테스트 권한</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MENU_AUTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMP_AUTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMPINFO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORG_CD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RANK_CD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IS_MALE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOB_NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDR_INFO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMAIL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HIRE_DT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LEAV_DT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMP_0001</t>
-  </si>
-  <si>
-    <t>ORG_0001</t>
-  </si>
-  <si>
-    <t>RANK_0001</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>주소</t>
-  </si>
-  <si>
-    <t>jtax90@naver.com</t>
-  </si>
-  <si>
-    <t>01077945147</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORG_NM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPPR_ORG_CD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORG_0002</t>
-  </si>
-  <si>
-    <t>ORG_0003</t>
-  </si>
-  <si>
-    <t>ORG_0004</t>
-  </si>
-  <si>
-    <t>000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RANK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자</t>
-  </si>
-  <si>
-    <t>RANK_0002</t>
-  </si>
-  <si>
-    <t>RANK_0003</t>
-  </si>
-  <si>
-    <t>RANK_NM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대표</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>팀장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주임</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RANK_0004</t>
-  </si>
-  <si>
-    <t>RANK_0005</t>
-  </si>
-  <si>
-    <t>RANK_0006</t>
-  </si>
-  <si>
-    <t>RANK_0007</t>
-  </si>
-  <si>
-    <t>RANK_0008</t>
-  </si>
-  <si>
-    <t>RANK_0009</t>
-  </si>
-  <si>
-    <t>RANK_0010</t>
-  </si>
-  <si>
-    <t>ORG_0005</t>
-  </si>
-  <si>
-    <t>ORG_0006</t>
-  </si>
-  <si>
-    <t>ORG_0007</t>
-  </si>
-  <si>
-    <t>ORG_0008</t>
-  </si>
-  <si>
-    <t>ORG_0009</t>
-  </si>
-  <si>
-    <t>ORG_0010</t>
-  </si>
-  <si>
-    <t>ORG_0011</t>
-  </si>
-  <si>
-    <t>경영지원부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인사부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>재무/회계부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마케팅부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영업부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기획부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>생산부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연구개발부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고객지원팀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정보시스템팀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>품질관리부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>법무팀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORG_0012</t>
-  </si>
-  <si>
-    <t>ORG_0013</t>
-  </si>
-  <si>
-    <t>COMMCODE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMMCODE_CD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMMCODE_NM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMMCODE_GCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USE</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>MENU_0017</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MENU_0019</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결재 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결재선 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>업무일지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PROC</t>
-  </si>
-  <si>
-    <t>진행</t>
-  </si>
-  <si>
-    <t>STAT</t>
-  </si>
-  <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>완료</t>
-  </si>
-  <si>
-    <t>STOP</t>
-  </si>
-  <si>
-    <t>보류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrStatsInqy1010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통계 조회 (사용 내역)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인카드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전도금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USE_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USE_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STAT_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STAT_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STAT_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEAV_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEAV_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEAV_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEAV_0040</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEAV_0050</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAY_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAY_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAY_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TYPE_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TYPE_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1024,15 +1205,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60644FAD-9B99-49D5-B453-33EA3359146C}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="15.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="21.625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="15.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="9" style="2"/>
@@ -1042,7 +1225,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1126,7 +1309,7 @@
       </c>
       <c r="H4" s="4"/>
       <c r="J4" s="3" t="str">
-        <f t="shared" ref="J4:J25" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"','"&amp;G4&amp;"','"&amp;H4&amp;"');"</f>
+        <f t="shared" ref="J4" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"','"&amp;G4&amp;"','"&amp;H4&amp;"');"</f>
         <v>INSERT INTO MENU VALUES('MENU_0002','0','공지사항','MENU_0001','intrBoardInqy2010.do','Y','2','');</v>
       </c>
     </row>
@@ -1138,24 +1321,24 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="G5" s="4">
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0003','0','일정관리','MENU_0001','intrScheInqy1010.do','Y','3','');</v>
+        <f t="shared" ref="J5:J32" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0003','0','FAQ','MENU_0001','intrFaqInqy2010.do','N','3','');</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1166,10 +1349,14 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>42</v>
       </c>
@@ -1178,8 +1365,8 @@
       </c>
       <c r="H6" s="4"/>
       <c r="J6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0004','0','전자결재','','','Y','4','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0004','0','일정관리','MENU_0001','intrScheInqy1010.do','Y','4','');</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1190,14 +1377,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
         <v>42</v>
       </c>
@@ -1206,8 +1389,8 @@
       </c>
       <c r="H7" s="4"/>
       <c r="J7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0005','0','결재 조회','MENU_0004','intrAprvInqy1010.do','Y','5','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0005','0','전자결재','','','Y','5','');</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1218,13 +1401,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>42</v>
@@ -1234,8 +1417,8 @@
       </c>
       <c r="H8" s="4"/>
       <c r="J8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0006','0','결재선 관리','MENU_0004','intrAprvInqy2010.do','Y','6','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0006','0','기안 작성','MENU_0005','intrAprvInqy1010.do','Y','6','');</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1246,10 +1429,14 @@
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+        <v>151</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
@@ -1258,8 +1445,8 @@
       </c>
       <c r="H9" s="4"/>
       <c r="J9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0007','0','업무관리','','','Y','7','');</v>
+        <f t="shared" ref="J9:J10" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0007','0','결재 조회','MENU_0005','intrAprvInqy2010.do','Y','7','');</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1270,24 +1457,24 @@
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="G10" s="4">
         <v>8</v>
       </c>
       <c r="H10" s="4"/>
       <c r="J10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0008','0','업무일지','MENU_0007','intrTaskInqy1010.do','Y','8','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO MENU VALUES('MENU_0008','0','결재선 관리','MENU_0005','intrAprvInqy3010.do','N','8','');</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1298,20 +1485,24 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+        <v>179</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>169</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="G11" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="4"/>
       <c r="J11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0009','0','인사정보','','','Y','9','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0009','0','잔여휴가 조회','MENU_0005','intrAprvInqy3010.do','N','8','');</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1322,14 +1513,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>42</v>
       </c>
@@ -1338,8 +1525,8 @@
       </c>
       <c r="H12" s="4"/>
       <c r="J12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0010','0','연락처','MENU_0009','intrEmpInqy2010.do','Y','10','');</v>
+        <f t="shared" ref="J12" si="3">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;D12&amp;"','"&amp;E12&amp;"','"&amp;F12&amp;"','"&amp;G12&amp;"','"&amp;H12&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0010','0','업무일지','','','Y','10','');</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1347,23 +1534,27 @@
         <v>24</v>
       </c>
       <c r="B13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="F13" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="4"/>
       <c r="J13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0011','1','공유정보 관리','','','Y','11','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0011','0','업무일지 작성','MENU_0010','intrTaskInqy1010.do','Y','10','');</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1371,27 +1562,23 @@
         <v>25</v>
       </c>
       <c r="B14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="4"/>
       <c r="J14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0012','1','공지사항 관리','MENU_0011','intrBoardInqy1010.do','Y','12','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0012','0','인사정보','','','Y','11','');</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1399,27 +1586,27 @@
         <v>26</v>
       </c>
       <c r="B15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="4"/>
       <c r="J15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0013','1','업무일지 조회','MENU_0011','intrTaskInqy2010.do','Y','13','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0013','0','연락처','MENU_0012','intrEmpInqy2010.do','Y','12','');</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1427,23 +1614,27 @@
         <v>27</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+        <v>163</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="F16" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="G16" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0014','1','결재 관리','','','Y','14','');</v>
+        <f t="shared" ref="J16" si="4">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0014','0','부서/직급 조회','MENU_0012','intrRoleInqy1010.do','N','13','');</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1454,24 +1645,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>61</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0015','1','기안문 관리','MENU_0014','intrTempInqy1010.do','Y','15','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0015','1','공유정보 관리','','','Y','14','');</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1482,24 +1669,24 @@
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="4"/>
       <c r="J18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0016','1','프로젝트 관리','MENU_0014','intrProjInqy1010.do','Y','16','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0016','1','공지사항 관리','MENU_0015','intrBoardInqy1010.do','Y','15','');</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1510,20 +1697,24 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="F19" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="G19" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="4"/>
       <c r="J19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0017','1','인사정보','','','Y','17','');</v>
+        <f t="shared" ref="J19:J20" si="5">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A19&amp;"','"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;D19&amp;"','"&amp;E19&amp;"','"&amp;F19&amp;"','"&amp;G19&amp;"','"&amp;H19&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0017','1','FAQ 관리','MENU_0015','intrFaqInqy1010.do','N','16','');</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1534,24 +1725,24 @@
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>62</v>
+        <v>187</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="G20" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H20" s="4"/>
       <c r="J20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0018','1','사원 관리','MENU_0017','intrEmpInqy1010.do','Y','18','');</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO MENU VALUES('MENU_0018','1','통계 조회 (사용 내역)','MENU_0015','intrStatsInqy1010.do','N','17','');</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1562,20 +1753,24 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="4"/>
       <c r="J21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0019','1','시스템 관리','','','Y','19','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0019','1','업무일지 조회','MENU_0015','intrTaskInqy2010.do','Y','18','');</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1586,24 +1781,20 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H22" s="4"/>
       <c r="J22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0020','1','권한 관리','MENU_0019','intrAuthInqy1010.do','Y','20','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0020','1','결재 관리','','','Y','19','');</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1614,80 +1805,268 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0021','1','메뉴 권한 부여','MENU_0019','intrAuthInqy2010.do','Y','21','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0021','1','양식 관리','MENU_0020','intrTempInqy1010.do','Y','20','');</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="4"/>
       <c r="J24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0022','1','사용자 권한 부여','MENU_0019','intrAuthInqy3010.do','Y','22','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0022','1','프로젝트 관리','MENU_0020','intrProjInqy1010.do','Y','21','');</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>73</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G25" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="4"/>
       <c r="J25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO MENU VALUES('MENU_0023','1','쿼리 입력','MENU_0019','intrQueryInqy1010.do','Y','23','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0023','1','인사정보','','','Y','22','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="4">
+        <v>23</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="J26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0024','1','사원 관리','MENU_0023','intrEmpInqy1010.do','Y','23','');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="4">
+        <v>24</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="J27" s="3" t="str">
+        <f t="shared" ref="J27" si="6">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A27&amp;"','"&amp;B27&amp;"','"&amp;C27&amp;"','"&amp;D27&amp;"','"&amp;E27&amp;"','"&amp;F27&amp;"','"&amp;G27&amp;"','"&amp;H27&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0025','1','메일 전송','MENU_0023','intrMailInqy1010.do','N','24','');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="4">
+        <v>25</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="J28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0026','1','시스템 관리','','','Y','25','');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="4">
+        <v>26</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="J29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0027','1','권한 관리','MENU_0026','intrAuthInqy1010.do','Y','26','');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="4">
+        <v>27</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="J30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0028','1','메뉴 권한 부여','MENU_0026','intrAuthInqy2010.do','Y','27','');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="4">
+        <v>28</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="J31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0029','1','사용자 권한 부여','MENU_0026','intrAuthInqy3010.do','Y','28','');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="4">
+        <v>29</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="J32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0030','1','쿼리 입력','MENU_0026','intrQueryInqy1010.do','Y','29','');</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +2084,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1716,7 +2095,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1761,10 +2140,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -1789,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBD6899-63FF-4260-80D6-0650038B0C85}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1803,7 +2182,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1861,7 +2240,7 @@
       </c>
       <c r="E4" s="4"/>
       <c r="G4" s="3" t="str">
-        <f t="shared" ref="G4:G25" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"');"</f>
+        <f t="shared" ref="G4:G30" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"');"</f>
         <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0002','Y','2','');</v>
       </c>
     </row>
@@ -2231,7 +2610,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>14</v>
@@ -2250,7 +2629,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>14</v>
@@ -2262,6 +2641,139 @@
       <c r="G25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0023','Y','23','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="4">
+        <v>24</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0024','Y','24','');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="4">
+        <v>25</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0025','Y','25','');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4">
+        <v>26</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="G28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0026','Y','26','');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4">
+        <v>27</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0027','Y','27','');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="4">
+        <v>28</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="G30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0028','Y','28','');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="4">
+        <v>29</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="G31" s="3" t="str">
+        <f t="shared" ref="G31" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A31&amp;"','"&amp;B31&amp;"','"&amp;C31&amp;"','"&amp;D31&amp;"','"&amp;E31&amp;"');"</f>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0029','Y','29','');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="4">
+        <v>30</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="G32" s="3" t="str">
+        <f t="shared" ref="G32" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A32&amp;"','"&amp;B32&amp;"','"&amp;C32&amp;"','"&amp;D32&amp;"','"&amp;E32&amp;"');"</f>
+        <v>INSERT INTO MENU_AUTH VALUES('AUTH_0001','MENU_0030','Y','30','');</v>
       </c>
     </row>
   </sheetData>
@@ -2289,7 +2801,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2359,7 +2871,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2379,28 +2891,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>2</v>
@@ -2409,43 +2921,43 @@
         <v>3</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L3" s="4">
         <v>20230814</v>
@@ -2484,7 +2996,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2496,13 +3008,13 @@
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
@@ -2522,17 +3034,17 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
         <v>20230814</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>42</v>
@@ -2548,17 +3060,17 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4">
         <v>20230814</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>42</v>
@@ -2574,17 +3086,17 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4">
         <v>20230814</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>42</v>
@@ -2600,17 +3112,17 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4">
         <v>20230814</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>42</v>
@@ -2626,17 +3138,17 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4">
         <v>20230814</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>42</v>
@@ -2652,17 +3164,17 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4">
         <v>20230814</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>42</v>
@@ -2678,17 +3190,17 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4">
         <v>20230814</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>42</v>
@@ -2704,17 +3216,17 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
         <v>20230814</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>42</v>
@@ -2730,17 +3242,17 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4">
         <v>20230814</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>42</v>
@@ -2756,17 +3268,17 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4">
         <v>20230814</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>42</v>
@@ -2782,17 +3294,17 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
         <v>20230814</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>42</v>
@@ -2808,17 +3320,17 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4">
         <v>20230814</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>42</v>
@@ -2834,17 +3346,17 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4">
         <v>20230814</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>42</v>
@@ -2886,7 +3398,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2897,10 +3409,10 @@
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
@@ -2920,16 +3432,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="4">
         <v>20230814</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>42</v>
@@ -2945,16 +3457,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4">
         <v>20230814</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>42</v>
@@ -2970,16 +3482,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4">
         <v>20230814</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>42</v>
@@ -2995,16 +3507,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C6" s="4">
         <v>20230814</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>42</v>
@@ -3020,16 +3532,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C7" s="4">
         <v>20230814</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>42</v>
@@ -3045,16 +3557,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C8" s="4">
         <v>20230814</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>42</v>
@@ -3070,16 +3582,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C9" s="4">
         <v>20230814</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>42</v>
@@ -3095,16 +3607,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C10" s="4">
         <v>20230814</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>42</v>
@@ -3120,16 +3632,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C11" s="4">
         <v>20230814</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>42</v>
@@ -3145,16 +3657,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C12" s="4">
         <v>20230814</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>42</v>
@@ -3182,10 +3694,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E19CE9-CDB6-46E2-AE0E-C80BE1FBF213}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3196,7 +3708,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3208,13 +3720,13 @@
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
@@ -3234,13 +3746,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>197</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D3" s="4">
         <v>20250520</v>
@@ -3257,18 +3769,18 @@
       <c r="H3" s="4"/>
       <c r="J3" s="3" t="str">
         <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('Y','Y','USE','20250520','80516','Y','1','');</v>
+        <v>INSERT INTO COMMCODE VALUES('USE_0010','Y','use','20250520','80516','Y','1','');</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D4" s="4">
         <v>20250520</v>
@@ -3285,18 +3797,18 @@
       <c r="H4" s="4"/>
       <c r="J4" s="3" t="str">
         <f t="shared" ref="J4" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"','"&amp;G4&amp;"','"&amp;H4&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('N','N','USE','20250520','80525','Y','2','');</v>
+        <v>INSERT INTO COMMCODE VALUES('USE_0020','N','use','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="D5" s="4">
         <v>20250520</v>
@@ -3313,18 +3825,18 @@
       <c r="H5" s="4"/>
       <c r="J5" s="3" t="str">
         <f t="shared" ref="J5:J6" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('PROC','진행','STAT','20250520','80525','Y','1','');</v>
+        <v>INSERT INTO COMMCODE VALUES('STAT_0010','진행','stat','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="D6" s="4">
         <v>20250520</v>
@@ -3341,18 +3853,18 @@
       <c r="H6" s="4"/>
       <c r="J6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO COMMCODE VALUES('END','완료','STAT','20250520','80525','Y','2','');</v>
+        <v>INSERT INTO COMMCODE VALUES('STAT_0020','완료','stat','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="D7" s="4">
         <v>20250520</v>
@@ -3369,7 +3881,287 @@
       <c r="H7" s="4"/>
       <c r="J7" s="3" t="str">
         <f t="shared" ref="J7" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;D7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('STOP','보류','STAT','20250520','80525','Y','3','');</v>
+        <v>INSERT INTO COMMCODE VALUES('STAT_0030','보류','stat','20250520','80525','Y','3','');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E8" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="J8" s="3" t="str">
+        <f t="shared" ref="J8:J12" si="3">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0010','연차','leav','20250520','80525','Y','1','');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E9" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="J9" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0020','병가','leav','20250520','80525','Y','2','');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E10" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0030','경조휴가','leav','20250520','80525','Y','3','');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E11" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="J11" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0040','반차','leav','20250520','80525','Y','4','');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E12" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="4">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="J12" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0050','기타','leav','20250520','80525','Y','5','');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E13" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="J13" s="3" t="str">
+        <f t="shared" ref="J13:J15" si="4">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;D13&amp;"','"&amp;E13&amp;"','"&amp;F13&amp;"','"&amp;G13&amp;"','"&amp;H13&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('PAY_0010','현금','pay','20250520','80525','Y','1','');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E14" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="J14" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO COMMCODE VALUES('PAY_0020','개인카드','pay','20250520','80525','Y','2','');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E15" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="J15" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO COMMCODE VALUES('PAY_0030','전도금','pay','20250520','80525','Y','3','');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E16" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="J16" s="3" t="str">
+        <f t="shared" ref="J16:J17" si="5">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('TYPE_0010','결재','type','20250520','80525','Y','1','');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E17" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="J17" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO COMMCODE VALUES('TYPE_0020','참조','type','20250520','80525','Y','2','');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# 작업 기간 - 2025-06-09 ~ 2025-06-14
# 커밋 내용
- 파일 다중처리 개발
- 프로필 이미지 업로드 기능 미작동 오류 수정
- 인사정보 재직여부 조회 오류 수정
- 결재선 화면 상 저장 기능 추가
- 결재선 팝업 화면 상 기능 개발
- 물품 등록 팝업 화면 상 기능 개발
- 정산내역 팝업 화면 상 기능 개발
- 결재 상세 화면 개발
- 결재선 조회 팝업 개발
- 회의 관리 화면 개발 (등록, 수정, 제거)
</commit_message>
<xml_diff>
--- a/02.프로젝트/01.인트라넷/01.설계/인트라넷 데이터.xlsx
+++ b/02.프로젝트/01.인트라넷/01.설계/인트라넷 데이터.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knn\Documents\hikr90\02.프로젝트\01.인트라넷\01.설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE7C38-9BBD-497E-9645-ADAC89AA8220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02348174-7B32-4D41-B636-458B9BEDC33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="793" activeTab="7" xr2:uid="{B204C4DA-9ED1-4F0A-AC7E-C11DE778500E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="216">
   <si>
     <t>EMP_IDX</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -559,10 +559,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>결재선 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>진행</t>
   </si>
   <si>
@@ -587,22 +583,6 @@
     <t>MENU_0024</t>
   </si>
   <si>
-    <t>FAQ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAQ 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메일 전송</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부서/직급 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MENU_0025</t>
   </si>
   <si>
@@ -619,30 +599,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>intrAprvInqy3010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intrFaqInqy2010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intrFaqInqy1010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intrMailInqy1010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intrRoleInqy1010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>업무일지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -651,13 +607,6 @@
   </si>
   <si>
     <t>MENU_0030</t>
-  </si>
-  <si>
-    <t>MENU_0030</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잔여휴가 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -689,10 +638,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>통계 조회 (사용 내역)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현금</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -713,22 +658,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>use</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>leav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pay</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>USE_0010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -789,8 +718,85 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>기안</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TYPE_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STEP_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STEP_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STEP_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결재진행중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결재완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결재반송</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intrMtgInqy1010.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통계 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회의관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USE</t>
+  </si>
+  <si>
+    <t>STAT</t>
+  </si>
+  <si>
+    <t>LEAV</t>
+  </si>
+  <si>
+    <t>PAY</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>REQ</t>
+  </si>
+  <si>
+    <t>STEP</t>
   </si>
 </sst>
 </file>
@@ -1205,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60644FAD-9B99-49D5-B453-33EA3359146C}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1321,24 +1327,24 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G5" s="4">
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="3" t="str">
-        <f t="shared" ref="J5:J32" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
-        <v>INSERT INTO MENU VALUES('MENU_0003','0','FAQ','MENU_0001','intrFaqInqy2010.do','N','3','');</v>
+        <f t="shared" ref="J5:J27" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0003','0','회의관리','MENU_0001','intrMtgInqy1010.do','Y','3','');</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1401,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
@@ -1445,7 +1451,7 @@
       </c>
       <c r="H9" s="4"/>
       <c r="J9" s="3" t="str">
-        <f t="shared" ref="J9:J10" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"');"</f>
+        <f t="shared" ref="J9" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"');"</f>
         <v>INSERT INTO MENU VALUES('MENU_0007','0','결재 조회','MENU_0005','intrAprvInqy2010.do','Y','7','');</v>
       </c>
     </row>
@@ -1457,24 +1463,20 @@
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4">
         <v>8</v>
       </c>
       <c r="H10" s="4"/>
       <c r="J10" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO MENU VALUES('MENU_0008','0','결재선 관리','MENU_0005','intrAprvInqy3010.do','N','8','');</v>
+        <f t="shared" ref="J10" si="3">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A10&amp;"','"&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;D10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"','"&amp;H10&amp;"');"</f>
+        <v>INSERT INTO MENU VALUES('MENU_0008','0','업무일지','','','Y','8','');</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1485,24 +1487,24 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H11" s="4"/>
       <c r="J11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0009','0','잔여휴가 조회','MENU_0005','intrAprvInqy3010.do','N','8','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0009','0','업무일지 작성','MENU_0008','intrTaskInqy1010.do','Y','9','');</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1513,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>175</v>
+        <v>51</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1525,8 +1527,8 @@
       </c>
       <c r="H12" s="4"/>
       <c r="J12" s="3" t="str">
-        <f t="shared" ref="J12" si="3">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;D12&amp;"','"&amp;E12&amp;"','"&amp;F12&amp;"','"&amp;G12&amp;"','"&amp;H12&amp;"');"</f>
-        <v>INSERT INTO MENU VALUES('MENU_0010','0','업무일지','','','Y','10','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0010','0','인사정보','','','Y','10','');</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1537,24 +1539,24 @@
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>168</v>
+        <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13" s="4"/>
       <c r="J13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0011','0','업무일지 작성','MENU_0010','intrTaskInqy1010.do','Y','10','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0011','0','연락처','MENU_0010','intrEmpInqy2010.do','Y','11','');</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1562,10 +1564,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1573,12 +1575,12 @@
         <v>42</v>
       </c>
       <c r="G14" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14" s="4"/>
       <c r="J14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0012','0','인사정보','','','Y','11','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0012','1','공유정보 관리','','','Y','12','');</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1586,27 +1588,27 @@
         <v>26</v>
       </c>
       <c r="B15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H15" s="4"/>
       <c r="J15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0013','0','연락처','MENU_0012','intrEmpInqy2010.do','Y','12','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0013','1','공지사항 관리','MENU_0012','intrBoardInqy1010.do','Y','13','');</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1614,27 +1616,27 @@
         <v>27</v>
       </c>
       <c r="B16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G16" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="3" t="str">
         <f t="shared" ref="J16" si="4">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
-        <v>INSERT INTO MENU VALUES('MENU_0014','0','부서/직급 조회','MENU_0012','intrRoleInqy1010.do','N','13','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0014','1','통계 조회','MENU_0012','intrStatsInqy1010.do','Y','14','');</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1645,20 +1647,24 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0015','1','공유정보 관리','','','Y','14','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0015','1','업무일지 조회','MENU_0012','intrTaskInqy2010.do','Y','15','');</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1669,24 +1675,20 @@
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" s="4"/>
       <c r="J18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0016','1','공지사항 관리','MENU_0015','intrBoardInqy1010.do','Y','15','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0016','1','결재 관리','','','Y','16','');</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1697,24 +1699,24 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>171</v>
+        <v>58</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G19" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H19" s="4"/>
       <c r="J19" s="3" t="str">
-        <f t="shared" ref="J19:J20" si="5">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A19&amp;"','"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;D19&amp;"','"&amp;E19&amp;"','"&amp;F19&amp;"','"&amp;G19&amp;"','"&amp;H19&amp;"');"</f>
-        <v>INSERT INTO MENU VALUES('MENU_0017','1','FAQ 관리','MENU_0015','intrFaqInqy1010.do','N','16','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0017','1','양식 관리','MENU_0016','intrTempInqy1010.do','Y','17','');</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1725,24 +1727,24 @@
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>186</v>
+        <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G20" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H20" s="4"/>
       <c r="J20" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>INSERT INTO MENU VALUES('MENU_0018','1','통계 조회 (사용 내역)','MENU_0015','intrStatsInqy1010.do','N','17','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0018','1','프로젝트 관리','MENU_0016','intrProjInqy1010.do','Y','18','');</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1753,24 +1755,20 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21" s="4"/>
       <c r="J21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0019','1','업무일지 조회','MENU_0015','intrTaskInqy2010.do','Y','18','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0019','1','인사정보','','','Y','19','');</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1781,20 +1779,24 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="F22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H22" s="4"/>
       <c r="J22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0020','1','결재 관리','','','Y','19','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0020','1','사원 관리','MENU_0019','intrEmpInqy1010.do','Y','20','');</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1805,24 +1807,20 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0021','1','양식 관리','MENU_0020','intrTempInqy1010.do','Y','20','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0021','1','시스템 관리','','','Y','21','');</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1833,24 +1831,24 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H24" s="4"/>
       <c r="J24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0022','1','프로젝트 관리','MENU_0020','intrProjInqy1010.do','Y','21','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0022','1','권한 관리','MENU_0021','intrAuthInqy1010.do','Y','22','');</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1861,212 +1859,80 @@
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="F25" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G25" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H25" s="4"/>
       <c r="J25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0023','1','인사정보','','','Y','22','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0023','1','메뉴 권한 부여','MENU_0021','intrAuthInqy2010.do','Y','23','');</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G26" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H26" s="4"/>
       <c r="J26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0024','1','사원 관리','MENU_0023','intrEmpInqy1010.do','Y','23','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0024','1','사용자 권한 부여','MENU_0021','intrAuthInqy3010.do','Y','24','');</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>172</v>
+        <v>70</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="G27" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H27" s="4"/>
       <c r="J27" s="3" t="str">
-        <f t="shared" ref="J27" si="6">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A27&amp;"','"&amp;B27&amp;"','"&amp;C27&amp;"','"&amp;D27&amp;"','"&amp;E27&amp;"','"&amp;F27&amp;"','"&amp;G27&amp;"','"&amp;H27&amp;"');"</f>
-        <v>INSERT INTO MENU VALUES('MENU_0025','1','메일 전송','MENU_0023','intrMailInqy1010.do','N','24','');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="4">
-        <v>25</v>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="J28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0026','1','시스템 관리','','','Y','25','');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="4">
-        <v>26</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="J29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0027','1','권한 관리','MENU_0026','intrAuthInqy1010.do','Y','26','');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="4">
-        <v>27</v>
-      </c>
-      <c r="H30" s="4"/>
-      <c r="J30" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0028','1','메뉴 권한 부여','MENU_0026','intrAuthInqy2010.do','Y','27','');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="4">
-        <v>28</v>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="J31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0029','1','사용자 권한 부여','MENU_0026','intrAuthInqy3010.do','Y','28','');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="4">
-        <v>29</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="J32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0030','1','쿼리 입력','MENU_0026','intrQueryInqy1010.do','Y','29','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0025','1','쿼리 입력','MENU_0021','intrQueryInqy1010.do','Y','25','');</v>
       </c>
     </row>
   </sheetData>
@@ -2648,7 +2514,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>14</v>
@@ -2667,7 +2533,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>14</v>
@@ -2686,7 +2552,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>14</v>
@@ -2705,7 +2571,7 @@
         <v>34</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>14</v>
@@ -2724,7 +2590,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>14</v>
@@ -2743,7 +2609,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>14</v>
@@ -2762,7 +2628,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>14</v>
@@ -3694,10 +3560,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E19CE9-CDB6-46E2-AE0E-C80BE1FBF213}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3746,13 +3612,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D3" s="4">
         <v>20250520</v>
@@ -3769,18 +3635,18 @@
       <c r="H3" s="4"/>
       <c r="J3" s="3" t="str">
         <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('USE_0010','Y','use','20250520','80516','Y','1','');</v>
+        <v>INSERT INTO COMMCODE VALUES('USE_0010','Y','USE','20250520','80516','Y','1','');</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D4" s="4">
         <v>20250520</v>
@@ -3796,19 +3662,19 @@
       </c>
       <c r="H4" s="4"/>
       <c r="J4" s="3" t="str">
-        <f t="shared" ref="J4" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"','"&amp;G4&amp;"','"&amp;H4&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('USE_0020','N','use','20250520','80525','Y','2','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"','"&amp;G4&amp;"','"&amp;H4&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('USE_0020','N','USE','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D5" s="4">
         <v>20250520</v>
@@ -3824,19 +3690,19 @@
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="3" t="str">
-        <f t="shared" ref="J5:J6" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('STAT_0010','진행','stat','20250520','80525','Y','1','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STAT_0010','진행','STAT','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D6" s="4">
         <v>20250520</v>
@@ -3852,19 +3718,19 @@
       </c>
       <c r="H6" s="4"/>
       <c r="J6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO COMMCODE VALUES('STAT_0020','완료','stat','20250520','80525','Y','2','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A6&amp;"','"&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STAT_0020','완료','STAT','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D7" s="4">
         <v>20250520</v>
@@ -3880,19 +3746,19 @@
       </c>
       <c r="H7" s="4"/>
       <c r="J7" s="3" t="str">
-        <f t="shared" ref="J7" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;D7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('STAT_0030','보류','stat','20250520','80525','Y','3','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;D7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STAT_0030','보류','STAT','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D8" s="4">
         <v>20250520</v>
@@ -3908,19 +3774,19 @@
       </c>
       <c r="H8" s="4"/>
       <c r="J8" s="3" t="str">
-        <f t="shared" ref="J8:J12" si="3">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('LEAV_0010','연차','leav','20250520','80525','Y','1','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0010','연차','LEAV','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D9" s="4">
         <v>20250520</v>
@@ -3936,19 +3802,19 @@
       </c>
       <c r="H9" s="4"/>
       <c r="J9" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO COMMCODE VALUES('LEAV_0020','병가','leav','20250520','80525','Y','2','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0020','병가','LEAV','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D10" s="4">
         <v>20250520</v>
@@ -3964,19 +3830,19 @@
       </c>
       <c r="H10" s="4"/>
       <c r="J10" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO COMMCODE VALUES('LEAV_0030','경조휴가','leav','20250520','80525','Y','3','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A10&amp;"','"&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;D10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"','"&amp;H10&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0030','경조휴가','LEAV','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D11" s="4">
         <v>20250520</v>
@@ -3992,19 +3858,19 @@
       </c>
       <c r="H11" s="4"/>
       <c r="J11" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO COMMCODE VALUES('LEAV_0040','반차','leav','20250520','80525','Y','4','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A11&amp;"','"&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;D11&amp;"','"&amp;E11&amp;"','"&amp;F11&amp;"','"&amp;G11&amp;"','"&amp;H11&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0040','반차','LEAV','20250520','80525','Y','4','');</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D12" s="4">
         <v>20250520</v>
@@ -4020,19 +3886,19 @@
       </c>
       <c r="H12" s="4"/>
       <c r="J12" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO COMMCODE VALUES('LEAV_0050','기타','leav','20250520','80525','Y','5','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;D12&amp;"','"&amp;E12&amp;"','"&amp;F12&amp;"','"&amp;G12&amp;"','"&amp;H12&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('LEAV_0050','기타','LEAV','20250520','80525','Y','5','');</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="D13" s="4">
         <v>20250520</v>
@@ -4048,19 +3914,19 @@
       </c>
       <c r="H13" s="4"/>
       <c r="J13" s="3" t="str">
-        <f t="shared" ref="J13:J15" si="4">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;D13&amp;"','"&amp;E13&amp;"','"&amp;F13&amp;"','"&amp;G13&amp;"','"&amp;H13&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('PAY_0010','현금','pay','20250520','80525','Y','1','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;D13&amp;"','"&amp;E13&amp;"','"&amp;F13&amp;"','"&amp;G13&amp;"','"&amp;H13&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('PAY_0010','현금','PAY','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="D14" s="4">
         <v>20250520</v>
@@ -4076,19 +3942,19 @@
       </c>
       <c r="H14" s="4"/>
       <c r="J14" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO COMMCODE VALUES('PAY_0020','개인카드','pay','20250520','80525','Y','2','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A14&amp;"','"&amp;B14&amp;"','"&amp;C14&amp;"','"&amp;D14&amp;"','"&amp;E14&amp;"','"&amp;F14&amp;"','"&amp;G14&amp;"','"&amp;H14&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('PAY_0020','개인카드','PAY','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="D15" s="4">
         <v>20250520</v>
@@ -4104,19 +3970,19 @@
       </c>
       <c r="H15" s="4"/>
       <c r="J15" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO COMMCODE VALUES('PAY_0030','전도금','pay','20250520','80525','Y','3','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A15&amp;"','"&amp;B15&amp;"','"&amp;C15&amp;"','"&amp;D15&amp;"','"&amp;E15&amp;"','"&amp;F15&amp;"','"&amp;G15&amp;"','"&amp;H15&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('PAY_0030','전도금','PAY','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D16" s="4">
         <v>20250520</v>
@@ -4132,19 +3998,19 @@
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="3" t="str">
-        <f t="shared" ref="J16:J17" si="5">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
-        <v>INSERT INTO COMMCODE VALUES('TYPE_0010','결재','type','20250520','80525','Y','1','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('TYPE_0010','기안','TYPE','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D17" s="4">
         <v>20250520</v>
@@ -4160,8 +4026,176 @@
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>INSERT INTO COMMCODE VALUES('TYPE_0020','참조','type','20250520','80525','Y','2','');</v>
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A17&amp;"','"&amp;B17&amp;"','"&amp;C17&amp;"','"&amp;D17&amp;"','"&amp;E17&amp;"','"&amp;F17&amp;"','"&amp;G17&amp;"','"&amp;H17&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('TYPE_0020','결재','TYPE','20250520','80525','Y','2','');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E18" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="J18" s="3" t="str">
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A18&amp;"','"&amp;B18&amp;"','"&amp;C18&amp;"','"&amp;D18&amp;"','"&amp;E18&amp;"','"&amp;F18&amp;"','"&amp;G18&amp;"','"&amp;H18&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('TYPE_0030','참조','TYPE','20250520','80525','Y','3','');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E19" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="J19" s="3" t="str">
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A19&amp;"','"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;D19&amp;"','"&amp;E19&amp;"','"&amp;F19&amp;"','"&amp;G19&amp;"','"&amp;H19&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('REQ_0010','반입','REQ','20250520','80525','Y','1','');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E20" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="J20" s="3" t="str">
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A20&amp;"','"&amp;B20&amp;"','"&amp;C20&amp;"','"&amp;D20&amp;"','"&amp;E20&amp;"','"&amp;F20&amp;"','"&amp;G20&amp;"','"&amp;H20&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('REQ_0020','반출','REQ','20250520','80525','Y','2','');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E21" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="J21" s="3" t="str">
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A21&amp;"','"&amp;B21&amp;"','"&amp;C21&amp;"','"&amp;D21&amp;"','"&amp;E21&amp;"','"&amp;F21&amp;"','"&amp;G21&amp;"','"&amp;H21&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STEP_0010','결재진행중','STEP','20250520','80525','Y','1','');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E22" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="J22" s="3" t="str">
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A22&amp;"','"&amp;B22&amp;"','"&amp;C22&amp;"','"&amp;D22&amp;"','"&amp;E22&amp;"','"&amp;F22&amp;"','"&amp;G22&amp;"','"&amp;H22&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STEP_0020','결재완료','STEP','20250520','80525','Y','2','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E23" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="4">
+        <v>3</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="J23" s="3" t="str">
+        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A23&amp;"','"&amp;B23&amp;"','"&amp;C23&amp;"','"&amp;D23&amp;"','"&amp;E23&amp;"','"&amp;F23&amp;"','"&amp;G23&amp;"','"&amp;H23&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STEP_0030','결재반송','STEP','20250520','80525','Y','3','');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# 작업 기간 - 2025-06-15 ~ 2025-06-20
# 커밋 내용
- 메인화면 디자인 변경 (아이콘 추가, 목록 클릭 시 상세 이동, 전체보기 기능 수정)
- 메인화면 캘린더 개발
- 클릭 시 회의 관리 화면 내 목록 조회
- 회의 관리 목록 클릭 시, 회의 상세 팝업 조회되도록 개발
- 일정 관리 이벤트 클릭 시, 휴가 일정 상세 팝업 개발
- 법인카드 정산서 기안 등록 문제 수정
- 권한 등록 버튼 CSS 문제로 인해 보이지 않는 문제 수정
- 결재 관련 버튼 생성
- 결재 기능 개발
</commit_message>
<xml_diff>
--- a/02.프로젝트/01.인트라넷/01.설계/인트라넷 데이터.xlsx
+++ b/02.프로젝트/01.인트라넷/01.설계/인트라넷 데이터.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knn\Documents\hikr90\02.프로젝트\01.인트라넷\01.설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02348174-7B32-4D41-B636-458B9BEDC33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55B2B21-68C9-47A0-988D-5C1F1EDA97D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="793" activeTab="7" xr2:uid="{B204C4DA-9ED1-4F0A-AC7E-C11DE778500E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="224">
   <si>
     <t>EMP_IDX</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -634,10 +634,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>intrStatsInqy1010.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현금</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -770,10 +766,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>통계 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회의관리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -797,6 +789,46 @@
   </si>
   <si>
     <t>STEP</t>
+  </si>
+  <si>
+    <t>STAT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSLT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSLT_0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSLT_0020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSLT_0030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>승인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반송</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STEP_0040</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결재취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1211,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60644FAD-9B99-49D5-B453-33EA3359146C}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1327,13 +1359,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>42</v>
@@ -1343,7 +1375,7 @@
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="3" t="str">
-        <f t="shared" ref="J5:J27" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
+        <f t="shared" ref="J5:J26" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
         <v>INSERT INTO MENU VALUES('MENU_0003','0','회의관리','MENU_0001','intrMtgInqy1010.do','Y','3','');</v>
       </c>
     </row>
@@ -1619,24 +1651,24 @@
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>207</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G16" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="3" t="str">
-        <f t="shared" ref="J16" si="4">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
-        <v>INSERT INTO MENU VALUES('MENU_0014','1','통계 조회','MENU_0012','intrStatsInqy1010.do','Y','14','');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO MENU VALUES('MENU_0014','1','업무일지 조회','MENU_0012','intrTaskInqy2010.do','Y','15','');</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1647,24 +1679,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0015','1','업무일지 조회','MENU_0012','intrTaskInqy2010.do','Y','15','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0015','1','결재 관리','','','Y','16','');</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1675,20 +1703,24 @@
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+        <v>156</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="F18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H18" s="4"/>
       <c r="J18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0016','1','결재 관리','','','Y','16','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0016','1','양식 관리','MENU_0015','intrTempInqy1010.do','Y','17','');</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1699,24 +1731,24 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G19" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H19" s="4"/>
       <c r="J19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0017','1','양식 관리','MENU_0016','intrTempInqy1010.do','Y','17','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0017','1','프로젝트 관리','MENU_0015','intrProjInqy1010.do','Y','18','');</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1727,24 +1759,20 @@
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>74</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G20" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H20" s="4"/>
       <c r="J20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0018','1','프로젝트 관리','MENU_0016','intrProjInqy1010.do','Y','18','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0018','1','인사정보','','','Y','19','');</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1755,20 +1783,24 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21" s="4"/>
       <c r="J21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0019','1','인사정보','','','Y','19','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0019','1','사원 관리','MENU_0018','intrEmpInqy1010.do','Y','20','');</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1779,24 +1811,20 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22" s="4"/>
       <c r="J22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0020','1','사원 관리','MENU_0019','intrEmpInqy1010.do','Y','20','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0020','1','시스템 관리','','','Y','21','');</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1807,20 +1835,24 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="F23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0021','1','시스템 관리','','','Y','21','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0021','1','권한 관리','MENU_0020','intrAuthInqy1010.do','Y','22','');</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1831,24 +1863,24 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H24" s="4"/>
       <c r="J24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0022','1','권한 관리','MENU_0021','intrAuthInqy1010.do','Y','22','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0022','1','메뉴 권한 부여','MENU_0020','intrAuthInqy2010.do','Y','23','');</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1859,24 +1891,24 @@
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G25" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H25" s="4"/>
       <c r="J25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0023','1','메뉴 권한 부여','MENU_0021','intrAuthInqy2010.do','Y','23','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0023','1','사용자 권한 부여','MENU_0020','intrAuthInqy3010.do','Y','24','');</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1887,52 +1919,24 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G26" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H26" s="4"/>
       <c r="J26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0024','1','사용자 권한 부여','MENU_0021','intrAuthInqy3010.do','Y','24','');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="4">
-        <v>25</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="J27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO MENU VALUES('MENU_0025','1','쿼리 입력','MENU_0021','intrQueryInqy1010.do','Y','25','');</v>
+        <v>INSERT INTO MENU VALUES('MENU_0024','1','쿼리 입력','MENU_0020','intrQueryInqy1010.do','Y','25','');</v>
       </c>
     </row>
   </sheetData>
@@ -3560,10 +3564,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E19CE9-CDB6-46E2-AE0E-C80BE1FBF213}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3612,13 +3616,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D3" s="4">
         <v>20250520</v>
@@ -3634,19 +3638,19 @@
       </c>
       <c r="H3" s="4"/>
       <c r="J3" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"');"</f>
+        <f t="shared" ref="J3:J23" si="0">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"');"</f>
         <v>INSERT INTO COMMCODE VALUES('USE_0010','Y','USE','20250520','80516','Y','1','');</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D4" s="4">
         <v>20250520</v>
@@ -3662,19 +3666,19 @@
       </c>
       <c r="H4" s="4"/>
       <c r="J4" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"','"&amp;G4&amp;"','"&amp;H4&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('USE_0020','N','USE','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>152</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D5" s="4">
         <v>20250520</v>
@@ -3690,19 +3694,19 @@
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('STAT_0010','진행','STAT','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>153</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D6" s="4">
         <v>20250520</v>
@@ -3718,19 +3722,19 @@
       </c>
       <c r="H6" s="4"/>
       <c r="J6" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A6&amp;"','"&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('STAT_0020','완료','STAT','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>154</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D7" s="4">
         <v>20250520</v>
@@ -3746,19 +3750,19 @@
       </c>
       <c r="H7" s="4"/>
       <c r="J7" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;D7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('STAT_0030','보류','STAT','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D8" s="4">
         <v>20250520</v>
@@ -3774,19 +3778,19 @@
       </c>
       <c r="H8" s="4"/>
       <c r="J8" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('LEAV_0010','연차','LEAV','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>168</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D9" s="4">
         <v>20250520</v>
@@ -3802,19 +3806,19 @@
       </c>
       <c r="H9" s="4"/>
       <c r="J9" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('LEAV_0020','병가','LEAV','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D10" s="4">
         <v>20250520</v>
@@ -3830,19 +3834,19 @@
       </c>
       <c r="H10" s="4"/>
       <c r="J10" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A10&amp;"','"&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;D10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"','"&amp;H10&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('LEAV_0030','경조휴가','LEAV','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>170</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D11" s="4">
         <v>20250520</v>
@@ -3858,19 +3862,19 @@
       </c>
       <c r="H11" s="4"/>
       <c r="J11" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A11&amp;"','"&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;D11&amp;"','"&amp;E11&amp;"','"&amp;F11&amp;"','"&amp;G11&amp;"','"&amp;H11&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('LEAV_0040','반차','LEAV','20250520','80525','Y','4','');</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>171</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D12" s="4">
         <v>20250520</v>
@@ -3886,19 +3890,19 @@
       </c>
       <c r="H12" s="4"/>
       <c r="J12" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;D12&amp;"','"&amp;E12&amp;"','"&amp;F12&amp;"','"&amp;G12&amp;"','"&amp;H12&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('LEAV_0050','기타','LEAV','20250520','80525','Y','5','');</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D13" s="4">
         <v>20250520</v>
@@ -3914,19 +3918,19 @@
       </c>
       <c r="H13" s="4"/>
       <c r="J13" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;D13&amp;"','"&amp;E13&amp;"','"&amp;F13&amp;"','"&amp;G13&amp;"','"&amp;H13&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('PAY_0010','현금','PAY','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D14" s="4">
         <v>20250520</v>
@@ -3942,19 +3946,19 @@
       </c>
       <c r="H14" s="4"/>
       <c r="J14" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A14&amp;"','"&amp;B14&amp;"','"&amp;C14&amp;"','"&amp;D14&amp;"','"&amp;E14&amp;"','"&amp;F14&amp;"','"&amp;G14&amp;"','"&amp;H14&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('PAY_0020','개인카드','PAY','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D15" s="4">
         <v>20250520</v>
@@ -3970,19 +3974,19 @@
       </c>
       <c r="H15" s="4"/>
       <c r="J15" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A15&amp;"','"&amp;B15&amp;"','"&amp;C15&amp;"','"&amp;D15&amp;"','"&amp;E15&amp;"','"&amp;F15&amp;"','"&amp;G15&amp;"','"&amp;H15&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('PAY_0030','전도금','PAY','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D16" s="4">
         <v>20250520</v>
@@ -3998,19 +4002,19 @@
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('TYPE_0010','기안','TYPE','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D17" s="4">
         <v>20250520</v>
@@ -4026,19 +4030,19 @@
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A17&amp;"','"&amp;B17&amp;"','"&amp;C17&amp;"','"&amp;D17&amp;"','"&amp;E17&amp;"','"&amp;F17&amp;"','"&amp;G17&amp;"','"&amp;H17&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('TYPE_0020','결재','TYPE','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D18" s="4">
         <v>20250520</v>
@@ -4054,19 +4058,19 @@
       </c>
       <c r="H18" s="4"/>
       <c r="J18" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A18&amp;"','"&amp;B18&amp;"','"&amp;C18&amp;"','"&amp;D18&amp;"','"&amp;E18&amp;"','"&amp;F18&amp;"','"&amp;G18&amp;"','"&amp;H18&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('TYPE_0030','참조','TYPE','20250520','80525','Y','3','');</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D19" s="4">
         <v>20250520</v>
@@ -4082,19 +4086,19 @@
       </c>
       <c r="H19" s="4"/>
       <c r="J19" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A19&amp;"','"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;D19&amp;"','"&amp;E19&amp;"','"&amp;F19&amp;"','"&amp;G19&amp;"','"&amp;H19&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('REQ_0010','반입','REQ','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D20" s="4">
         <v>20250520</v>
@@ -4110,19 +4114,19 @@
       </c>
       <c r="H20" s="4"/>
       <c r="J20" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A20&amp;"','"&amp;B20&amp;"','"&amp;C20&amp;"','"&amp;D20&amp;"','"&amp;E20&amp;"','"&amp;F20&amp;"','"&amp;G20&amp;"','"&amp;H20&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('REQ_0020','반출','REQ','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D21" s="4">
         <v>20250520</v>
@@ -4138,19 +4142,19 @@
       </c>
       <c r="H21" s="4"/>
       <c r="J21" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A21&amp;"','"&amp;B21&amp;"','"&amp;C21&amp;"','"&amp;D21&amp;"','"&amp;E21&amp;"','"&amp;F21&amp;"','"&amp;G21&amp;"','"&amp;H21&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('STEP_0010','결재진행중','STEP','20250520','80525','Y','1','');</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D22" s="4">
         <v>20250520</v>
@@ -4166,19 +4170,19 @@
       </c>
       <c r="H22" s="4"/>
       <c r="J22" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A22&amp;"','"&amp;B22&amp;"','"&amp;C22&amp;"','"&amp;D22&amp;"','"&amp;E22&amp;"','"&amp;F22&amp;"','"&amp;G22&amp;"','"&amp;H22&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('STEP_0020','결재완료','STEP','20250520','80525','Y','2','');</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D23" s="4">
         <v>20250520</v>
@@ -4194,8 +4198,120 @@
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="3" t="str">
-        <f>"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A23&amp;"','"&amp;B23&amp;"','"&amp;C23&amp;"','"&amp;D23&amp;"','"&amp;E23&amp;"','"&amp;F23&amp;"','"&amp;G23&amp;"','"&amp;H23&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO COMMCODE VALUES('STEP_0030','결재반송','STEP','20250520','80525','Y','3','');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E24" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="4">
+        <v>4</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="J24" s="3" t="str">
+        <f t="shared" ref="J24" si="1">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A24&amp;"','"&amp;B24&amp;"','"&amp;C24&amp;"','"&amp;D24&amp;"','"&amp;E24&amp;"','"&amp;F24&amp;"','"&amp;G24&amp;"','"&amp;H24&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('STEP_0040','결재취소','STEP','20250520','80525','Y','4','');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E25" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="J25" s="3" t="str">
+        <f t="shared" ref="J25:J26" si="2">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A25&amp;"','"&amp;B25&amp;"','"&amp;C25&amp;"','"&amp;D25&amp;"','"&amp;E25&amp;"','"&amp;F25&amp;"','"&amp;G25&amp;"','"&amp;H25&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('RSLT_0010','승인','RSLT','20250520','80525','Y','1','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E26" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="J26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO COMMCODE VALUES('RSLT_0020','반송','RSLT','20250520','80525','Y','2','');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="4">
+        <v>20250520</v>
+      </c>
+      <c r="E27" s="4">
+        <v>80525</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="4">
+        <v>3</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="J27" s="3" t="str">
+        <f t="shared" ref="J27" si="3">"INSERT INTO "&amp;$A$1&amp;" VALUES('"&amp;A27&amp;"','"&amp;B27&amp;"','"&amp;C27&amp;"','"&amp;D27&amp;"','"&amp;E27&amp;"','"&amp;F27&amp;"','"&amp;G27&amp;"','"&amp;H27&amp;"');"</f>
+        <v>INSERT INTO COMMCODE VALUES('RSLT_0030','취소','RSLT','20250520','80525','Y','3','');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>